<commit_message>
test vtc, basic load test, bmpn model
</commit_message>
<xml_diff>
--- a/MatricesdePrueba.xlsx
+++ b/MatricesdePrueba.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Segurodeviajemundial" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t xml:space="preserve">Id </t>
   </si>
@@ -51,9 +51,6 @@
     <t>Comentarios</t>
   </si>
   <si>
-    <t>Cotizacion</t>
-  </si>
-  <si>
     <t>Mail de Cotizacion</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>SDVM_005</t>
   </si>
   <si>
-    <t>Eleccion del plan de visado</t>
-  </si>
-  <si>
     <t>VTC_001</t>
   </si>
   <si>
@@ -93,12 +87,6 @@
     <t>VTC_004</t>
   </si>
   <si>
-    <t>Matriz de Prueba SDVM (Caja Negra)</t>
-  </si>
-  <si>
-    <t>Matriz de Prueba VTC (Caja Blanca)</t>
-  </si>
-  <si>
     <t>Solicitar Cotizacion</t>
   </si>
   <si>
@@ -414,6 +402,95 @@
   </si>
   <si>
     <t>1 - El mail de cotizacion incluye un enlace que lleva la web, se debe confirmar esta redireccion</t>
+  </si>
+  <si>
+    <t>Recibir mail de Cotizacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Ingresar a https://pe.visatravelcenter.com/                                                                                                                      2 - Completar el formulario de cotizacion                                                                         3 - Clickear en el boton "Quiero mi asesoria"     </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Formulario:                                    Pais                                                   Nombre                                       Correo                                            Telefono   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                            </t>
+    </r>
+  </si>
+  <si>
+    <t>El usuario recibe un correo con los detalles de su cotizacion</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Por definir</t>
+  </si>
+  <si>
+    <t>Se esperaba que el correo se enviara al completar el formulario, tal como ocurre en las pruebas de SDVM, sin embargo no ocurre de esta manera. Se espera confirmacion de proceso</t>
+  </si>
+  <si>
+    <t>VTC_005</t>
+  </si>
+  <si>
+    <t>Eleccion del plan de visado - Estudio de perfil</t>
+  </si>
+  <si>
+    <t>Eleccion del plan de visado - Asesoría migratoria completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matriz de Prueba SDVM </t>
+  </si>
+  <si>
+    <t>Matriz de Prueba VTC</t>
+  </si>
+  <si>
+    <t>Al solicitar una cotizacion el usuario puede visualizar y elegir la opcion de Estudio de perfil en 30$</t>
+  </si>
+  <si>
+    <t>Al solicitar una cotizacion el usuario puede visualizar y elegir la opcion de Asesoría migratoria completa en 180$</t>
+  </si>
+  <si>
+    <t>1 - Solicitar una asesoria/conciliacion                              2 - Visualizar planes                         3 - Dar click en "Seleccionar" para la opcion Estudio de perfil</t>
+  </si>
+  <si>
+    <t>VTC_006</t>
+  </si>
+  <si>
+    <t>Seleccion metodo de pago</t>
+  </si>
+  <si>
+    <t>El usuario indica su metodo de pago y es dirigido a la plataforma de pago correspondiente</t>
+  </si>
+  <si>
+    <t>1 - Solicitar una asesoria/conciliacion                              2 - Visualizar planes                         3 - Dar click en "Seleccionar" para la opcion Asesoría migratoria completa</t>
+  </si>
+  <si>
+    <t>1 - Solicitar una asesoria/conciliacion                              2 - Seleccionar un plan de visado                                                          3 - Visualizar y seleccionar los metodos de pago                                    4 - Aceptar los terminos y condiciones                                             5 - Dar click en Pagar                            6 - Confirmar redireccion a plataforma de pago</t>
+  </si>
+  <si>
+    <t>VTC_001                       VTC_003                       VTC_004</t>
+  </si>
+  <si>
+    <t>El usuario completa su compra dentro de la plataforma de pago</t>
+  </si>
+  <si>
+    <t>VTC_001                       VTC_003                       VTC_004                             VTC_005</t>
   </si>
 </sst>
 </file>
@@ -477,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -546,13 +623,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -614,32 +699,102 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -776,6 +931,27 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de tabla 1" pivot="0" count="0"/>
@@ -792,10 +968,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="E2:E11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="E2:E11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="E2:E11"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Resultado obtenido" dataDxfId="6"/>
+    <tableColumn id="1" name="Resultado obtenido" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="Estilo de tabla 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="E2:E8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="E2:E8"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Resultado obtenido" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de tabla 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1066,9 +1252,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,350 +1271,350 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="9" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="8"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" s="3" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" s="3" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="10" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="3" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" s="3" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="E11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="3" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"Correcto"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"No Ejecutado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1447,11 +1633,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,121 +1653,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="A1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="C8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="E3:E8">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Correcto"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="E3:E8">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"No Ejecutado"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
       <formula1>"Correcto, Error, No Ejecutado"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>